<commit_message>
new file:   core/checking.py 	modified:   core/model_config.py 	modified:   core/output_format_conversion.py 	modified:   core/struc_chain.py 	modified:   core/tagging_chain.py 	modified:   output_parser/tagging_inquiry_letter.py 	modified:   prompt/annual_report.py 	modified:   prompt/tagging.py 	modified:   requirements.txt 	modified:   vector_store/Milvus.py
</commit_message>
<xml_diff>
--- a/docs/标签规则/规则定义/严重性.xlsx
+++ b/docs/标签规则/规则定义/严重性.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataKiller\DataKiller 1.0\docs\标签规则\规则定义\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8A36D0-D67A-4AE4-A079-3CC97870ECD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8535A6D3-24D2-4C06-B282-133ECFFED201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3773" yWindow="1890" windowWidth="14400" windowHeight="8722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4433" yWindow="2310" windowWidth="14400" windowHeight="9128" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,11 +31,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>严重性指该问题产生后果的严重程度。
+    <t>"严重性指该问题产生后果的严重程度。
 满足下述任一维度，该问题即被判定为”严重性等级高“：
-维度1-合规性风险，包括如“内部控制制度、是否符合相关制度、是否履行必要的审议程序、管理层是否勤勉尽责、是否损害投资者利益”等词
-维度2-经营性风险，包括如“持续经营能力、终止上市风险、是否影响日常经营业务开展”等词
-问询问题内容既不涉及合规性风险，也不涉及经营性风险，仅涉及单个事件，则该问题被判定为”严重性等级低“。</t>
+维度1-合规性风险，包括如“内部控制制度、是否符合相关制度、是否履行必要的审议程序、全面梳理、管理层是否勤勉尽责、是否损害投资者利益”等词
+维度2-经营性风险，包括如“持续经营能力、终止上市风险、是否影响日常经营业务开展、退市风险”等词
+维度3-重大偏离风险，监管机构对问题的描述存在“重大不确定性、远高于、远低于、大幅增长、大幅下降“等这类副词"
+问询问题内容既不涉及合规性风险，也不涉及经营性风险和重大偏离风险，则该问题被判定为”严重性等级低“。
+**返回结果请从["严重性等级高", "严重性等级低"]中枚举**</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -378,7 +380,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -388,8 +390,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:1" ht="409.5" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>